<commit_message>
visual pie&word cloud component
</commit_message>
<xml_diff>
--- a/TimeVisual/data/gatte-test.xlsx
+++ b/TimeVisual/data/gatte-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB8C0DE-66DF-4AED-9E3B-F99EBB010777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4478C27B-4B84-4310-85B7-00384A66D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="1905" windowWidth="15165" windowHeight="11235" firstSheet="21" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10050" yWindow="1560" windowWidth="15165" windowHeight="11235" firstSheet="21" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="305">
   <si>
     <t>起始</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1256,6 +1256,10 @@
   </si>
   <si>
     <t>data-code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visual-code</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -15889,7 +15893,7 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -15928,7 +15932,7 @@
         <v>302</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D38" si="0">INT(ABS(B2-A2)*1440)</f>
+        <f t="shared" ref="D2:D12" si="0">INT(ABS(B2-A2)*1440)</f>
         <v>39</v>
       </c>
     </row>
@@ -15966,40 +15970,129 @@
       <c r="A5" s="5">
         <v>44410.59375</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5">
+        <v>44410.627083333333</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="5">
+        <v>44410.63958333333</v>
+      </c>
+      <c r="B6" s="5">
+        <v>44410.65625</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="5">
+        <v>44410.660416666666</v>
+      </c>
+      <c r="B7" s="5">
+        <v>44410.679861111108</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="5">
+        <v>44410.688194444447</v>
+      </c>
+      <c r="B8" s="5">
+        <v>44410.729166666664</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="5">
+        <v>44410.881944444445</v>
+      </c>
+      <c r="B9" s="5">
+        <v>44410.920138888891</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="5">
+        <v>44410.925000000003</v>
+      </c>
+      <c r="B10" s="5">
+        <v>44410.943055555559</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="5">
+        <v>44410.95</v>
+      </c>
+      <c r="B11" s="5">
+        <v>44410.976388888892</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="5">
+        <v>44411.356944444444</v>
+      </c>
+      <c r="B12" s="5">
+        <v>44411.363194444442</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>44411.371527777781</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>

</xml_diff>